<commit_message>
fill team plan sheet
</commit_message>
<xml_diff>
--- a/phase 3/Phase 3-Team Planning.xlsx
+++ b/phase 3/Phase 3-Team Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YZN\Desktop\uOttawa_Teaching\CSI4142\Project\Phases_3+4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39d0109d20b3edff/Desktop/CSI4142/DataMing/phase 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9A2087-2FF6-4650-902C-F2A45B51A59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{BE9A2087-2FF6-4650-902C-F2A45B51A59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7336981-D5B6-4F64-92F7-BC4DD8DA8805}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC7B5491-6718-42D3-AD60-469765C6A1D2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BC7B5491-6718-42D3-AD60-469765C6A1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Deliverable checklist</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>CSI4142 - Project 2023</t>
+  </si>
+  <si>
+    <t>Chentao Jin</t>
   </si>
 </sst>
 </file>
@@ -199,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -223,6 +226,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,9 +247,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +287,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -387,7 +393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,7 +535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -540,28 +546,28 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="28" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
@@ -584,7 +590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
@@ -599,7 +605,7 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -610,84 +616,154 @@
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D9" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D10" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D11" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D12" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D13" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D14" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D15" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -696,7 +772,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -707,49 +783,89 @@
       <c r="F17" s="2"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D18" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D19" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.3</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D20" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="9">
+        <v>45386</v>
+      </c>
+      <c r="D21" s="9">
+        <v>45387</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -757,7 +873,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>